<commit_message>
individual del_c fixed in healthy part
</commit_message>
<xml_diff>
--- a/original_files/LEA/LEA.xlsx
+++ b/original_files/LEA/LEA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="700" windowWidth="20740" windowHeight="12840" tabRatio="677" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14120" tabRatio="677" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="h_gem_b1" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="h_gem_d2" sheetId="5" r:id="rId4"/>
     <sheet name="h_gem_del_a1" sheetId="6" r:id="rId5"/>
     <sheet name="h_gem_del_a2" sheetId="7" r:id="rId6"/>
-    <sheet name="gem_del_c1" sheetId="8" r:id="rId7"/>
+    <sheet name="h_gem_del_c1" sheetId="8" r:id="rId7"/>
     <sheet name="gem_ob_e1" sheetId="9" r:id="rId8"/>
     <sheet name="gem_ob_e2" sheetId="10" r:id="rId9"/>
     <sheet name="gem_ob_f1" sheetId="11" r:id="rId10"/>
@@ -8655,7 +8655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -23450,7 +23450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -51124,8 +51124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>